<commit_message>
Fix PSM matching: implement matching without replacement
修正PSM匹配逻辑：实现无放回匹配

关键修正:
1. 实现无放回匹配（Matching Without Replacement）
   - 每个对照组只能匹配一次
   - 匹配后立即从备选池移除
   - 确保每个城市权重相等

2. 优化卡尺设定
   - 从固定值0.05改为0.25 × 倾向得分标准差
   - 新卡尺: 0.0461
   - 符合学术规范

3. 匹配结果改进
   - 匹配率: 76.15% (83/109对)
   - 所有4个变量全部通过平衡性检验！
   - 平衡性: 4/4 (之前2/4)
   - 匹配后样本: 166个城市，2822条观测

4. 平衡性检验对比
   变量                    标准化差异
   ln_real_gdp:           8.15% (之前16.75%) ✓
   ln_人口密度:           5.37% ✓
   ln_金融发展水平:        6.40% ✓
   第二产业占GDP比重:     7.44% (之前12.98%) ✓

5. 学术优势
   - 无需复杂的加权最小二乘法（WLS）调整
   - 可直接使用标准固定效应DID模型
   - 回归结果无偏且符合学术规范

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/PSM_Baseline_2009/balance_check_results.xlsx
+++ b/PSM_Baseline_2009/balance_check_results.xlsx
@@ -467,17 +467,17 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.7341126481341</v>
+        <v>6.438261300782886</v>
       </c>
       <c r="C2" t="n">
-        <v>6.881414641238369</v>
+        <v>6.501110433718534</v>
       </c>
       <c r="D2" t="n">
-        <v>16.74571909376607</v>
+        <v>8.145282382069622</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -488,13 +488,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.902226740283599</v>
+        <v>5.722068186375838</v>
       </c>
       <c r="C3" t="n">
-        <v>5.942152692583337</v>
+        <v>5.768180621157776</v>
       </c>
       <c r="D3" t="n">
-        <v>4.767610181879959</v>
+        <v>5.370774989784516</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -509,13 +509,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7596661244752002</v>
+        <v>0.6021899870632997</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7149104020614996</v>
+        <v>0.5812001176826126</v>
       </c>
       <c r="D4" t="n">
-        <v>9.823355709457154</v>
+        <v>6.398799704345692</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -530,17 +530,17 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4913768879553982</v>
+        <v>0.497744963449168</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5034319341516941</v>
+        <v>0.4903009433128748</v>
       </c>
       <c r="D5" t="n">
-        <v>12.98125558292268</v>
+        <v>7.43668508647872</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>

</xml_diff>